<commit_message>
Added link to source in AQI dataset, removed cell highlights that were not necessary
</commit_message>
<xml_diff>
--- a/Data/Raw/US Census - Median Household Income 2020.xlsx
+++ b/Data/Raw/US Census - Median Household Income 2020.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69286B5-D548-4944-8BC1-51D0F0CC5C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D1F389-95A9-4DA7-AB10-C87952454D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="500" windowWidth="28900" windowHeight="15660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2820" yWindow="2820" windowWidth="17280" windowHeight="9960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="1" r:id="rId1"/>
@@ -2102,18 +2102,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -2172,20 +2166,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2577,2487 +2571,2244 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25" style="1" customWidth="1"/>
     <col min="2" max="2" width="80" style="1" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="7"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-    </row>
-    <row r="5" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+    </row>
+    <row r="5" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="10"/>
-    </row>
-    <row r="6" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="8"/>
+    </row>
+    <row r="6" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="10"/>
-    </row>
-    <row r="7" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C6" s="8"/>
+    </row>
+    <row r="7" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="10"/>
-    </row>
-    <row r="8" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="8"/>
+    </row>
+    <row r="8" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="10"/>
-    </row>
-    <row r="9" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C8" s="8"/>
+    </row>
+    <row r="9" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="10"/>
-    </row>
-    <row r="10" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="8"/>
+    </row>
+    <row r="10" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="10"/>
-    </row>
-    <row r="11" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="8"/>
+    </row>
+    <row r="11" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="10"/>
-    </row>
-    <row r="12" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C11" s="8"/>
+    </row>
+    <row r="12" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="10"/>
-    </row>
-    <row r="13" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C12" s="8"/>
+    </row>
+    <row r="13" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="10"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-    </row>
-    <row r="15" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C13" s="8"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+    </row>
+    <row r="15" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="10"/>
-    </row>
-    <row r="16" spans="1:3" ht="25.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="8"/>
+    </row>
+    <row r="16" spans="1:3" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="10"/>
-    </row>
-    <row r="17" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C16" s="8"/>
+    </row>
+    <row r="17" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="10"/>
-    </row>
-    <row r="18" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C17" s="8"/>
+    </row>
+    <row r="18" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="10"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-    </row>
-    <row r="20" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C18" s="8"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+    </row>
+    <row r="20" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="10"/>
-    </row>
-    <row r="21" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C20" s="8"/>
+    </row>
+    <row r="21" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="10"/>
-    </row>
-    <row r="22" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C21" s="8"/>
+    </row>
+    <row r="22" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="10"/>
-    </row>
-    <row r="23" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C22" s="8"/>
+    </row>
+    <row r="23" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="10"/>
-    </row>
-    <row r="24" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C23" s="8"/>
+    </row>
+    <row r="24" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="10"/>
-    </row>
-    <row r="25" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C24" s="8"/>
+    </row>
+    <row r="25" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="10"/>
-    </row>
-    <row r="26" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C25" s="8"/>
+    </row>
+    <row r="26" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="10"/>
-    </row>
-    <row r="27" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C26" s="8"/>
+    </row>
+    <row r="27" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="10"/>
-    </row>
-    <row r="28" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C27" s="8"/>
+    </row>
+    <row r="28" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="10"/>
-    </row>
-    <row r="29" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C28" s="8"/>
+    </row>
+    <row r="29" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C29" s="10"/>
-    </row>
-    <row r="30" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C29" s="8"/>
+    </row>
+    <row r="30" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C30" s="10"/>
-    </row>
-    <row r="31" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C30" s="8"/>
+    </row>
+    <row r="31" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C31" s="10"/>
-    </row>
-    <row r="32" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C31" s="8"/>
+    </row>
+    <row r="32" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="10"/>
-    </row>
-    <row r="33" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C32" s="8"/>
+    </row>
+    <row r="33" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C33" s="10"/>
-    </row>
-    <row r="34" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C33" s="8"/>
+    </row>
+    <row r="34" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C34" s="10"/>
-    </row>
-    <row r="35" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C34" s="8"/>
+    </row>
+    <row r="35" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C35" s="10"/>
-    </row>
-    <row r="36" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C35" s="8"/>
+    </row>
+    <row r="36" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C36" s="10"/>
-    </row>
-    <row r="37" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C36" s="8"/>
+    </row>
+    <row r="37" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B37" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C37" s="10"/>
-    </row>
-    <row r="38" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C37" s="8"/>
+    </row>
+    <row r="38" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C38" s="10"/>
-    </row>
-    <row r="39" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C38" s="8"/>
+    </row>
+    <row r="39" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B39" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C39" s="10"/>
-    </row>
-    <row r="40" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C39" s="8"/>
+    </row>
+    <row r="40" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B40" s="10" t="s">
+      <c r="B40" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C40" s="10"/>
-    </row>
-    <row r="41" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C40" s="8"/>
+    </row>
+    <row r="41" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B41" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C41" s="10"/>
-    </row>
-    <row r="42" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C41" s="8"/>
+    </row>
+    <row r="42" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C42" s="10"/>
-    </row>
-    <row r="43" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C42" s="8"/>
+    </row>
+    <row r="43" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B43" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C43" s="10"/>
-    </row>
-    <row r="44" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C43" s="8"/>
+    </row>
+    <row r="44" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="B44" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C44" s="10"/>
-    </row>
-    <row r="45" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C44" s="8"/>
+    </row>
+    <row r="45" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C45" s="10"/>
-    </row>
-    <row r="46" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C45" s="8"/>
+    </row>
+    <row r="46" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="B46" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C46" s="10"/>
-    </row>
-    <row r="47" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C46" s="8"/>
+    </row>
+    <row r="47" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="B47" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C47" s="10"/>
-    </row>
-    <row r="48" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C47" s="8"/>
+    </row>
+    <row r="48" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B48" s="10" t="s">
+      <c r="B48" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C48" s="10"/>
-    </row>
-    <row r="49" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C48" s="8"/>
+    </row>
+    <row r="49" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B49" s="10" t="s">
+      <c r="B49" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C49" s="10"/>
-    </row>
-    <row r="50" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C49" s="8"/>
+    </row>
+    <row r="50" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B50" s="10" t="s">
+      <c r="B50" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="10"/>
-    </row>
-    <row r="51" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C50" s="8"/>
+    </row>
+    <row r="51" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B51" s="10" t="s">
+      <c r="B51" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C51" s="10"/>
-    </row>
-    <row r="52" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C51" s="8"/>
+    </row>
+    <row r="52" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B52" s="10" t="s">
+      <c r="B52" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C52" s="10"/>
-    </row>
-    <row r="53" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C52" s="8"/>
+    </row>
+    <row r="53" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B53" s="10" t="s">
+      <c r="B53" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C53" s="10"/>
-    </row>
-    <row r="54" spans="1:3" ht="25.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C53" s="8"/>
+    </row>
+    <row r="54" spans="1:3" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B54" s="10" t="s">
+      <c r="B54" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C54" s="10"/>
-    </row>
-    <row r="55" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C54" s="8"/>
+    </row>
+    <row r="55" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B55" s="10" t="s">
+      <c r="B55" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C55" s="10"/>
-    </row>
-    <row r="56" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C55" s="8"/>
+    </row>
+    <row r="56" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B56" s="10" t="s">
+      <c r="B56" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C56" s="10"/>
-    </row>
-    <row r="57" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C56" s="8"/>
+    </row>
+    <row r="57" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B57" s="10" t="s">
+      <c r="B57" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C57" s="10"/>
-    </row>
-    <row r="58" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C57" s="8"/>
+    </row>
+    <row r="58" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B58" s="10" t="s">
+      <c r="B58" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C58" s="10"/>
-    </row>
-    <row r="59" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C58" s="8"/>
+    </row>
+    <row r="59" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B59" s="10" t="s">
+      <c r="B59" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C59" s="10"/>
-    </row>
-    <row r="60" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C59" s="8"/>
+    </row>
+    <row r="60" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B60" s="10" t="s">
+      <c r="B60" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C60" s="10"/>
-    </row>
-    <row r="61" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C60" s="8"/>
+    </row>
+    <row r="61" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B61" s="10" t="s">
+      <c r="B61" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C61" s="10"/>
-    </row>
-    <row r="62" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C61" s="8"/>
+    </row>
+    <row r="62" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B62" s="10" t="s">
+      <c r="B62" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C62" s="10"/>
-    </row>
-    <row r="63" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C62" s="8"/>
+    </row>
+    <row r="63" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B63" s="10" t="s">
+      <c r="B63" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C63" s="10"/>
-    </row>
-    <row r="64" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C63" s="8"/>
+    </row>
+    <row r="64" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B64" s="10" t="s">
+      <c r="B64" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C64" s="10"/>
-    </row>
-    <row r="65" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C64" s="8"/>
+    </row>
+    <row r="65" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B65" s="10" t="s">
+      <c r="B65" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="C65" s="10"/>
-    </row>
-    <row r="66" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C65" s="8"/>
+    </row>
+    <row r="66" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B66" s="10" t="s">
+      <c r="B66" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C66" s="10"/>
-    </row>
-    <row r="67" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C66" s="8"/>
+    </row>
+    <row r="67" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B67" s="10" t="s">
+      <c r="B67" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C67" s="10"/>
-    </row>
-    <row r="68" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C67" s="8"/>
+    </row>
+    <row r="68" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B68" s="10" t="s">
+      <c r="B68" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C68" s="10"/>
-    </row>
-    <row r="69" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C68" s="8"/>
+    </row>
+    <row r="69" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B69" s="10" t="s">
+      <c r="B69" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C69" s="10"/>
-    </row>
-    <row r="70" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C69" s="8"/>
+    </row>
+    <row r="70" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B70" s="10" t="s">
+      <c r="B70" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C70" s="10"/>
-    </row>
-    <row r="71" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C70" s="8"/>
+    </row>
+    <row r="71" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B71" s="10" t="s">
+      <c r="B71" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C71" s="10"/>
-    </row>
-    <row r="72" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C71" s="8"/>
+    </row>
+    <row r="72" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B72" s="10" t="s">
+      <c r="B72" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C72" s="10"/>
-    </row>
-    <row r="73" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C72" s="8"/>
+    </row>
+    <row r="73" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B73" s="10" t="s">
+      <c r="B73" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C73" s="10"/>
-    </row>
-    <row r="74" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C73" s="8"/>
+    </row>
+    <row r="74" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B74" s="10" t="s">
+      <c r="B74" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C74" s="10"/>
-    </row>
-    <row r="75" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C74" s="8"/>
+    </row>
+    <row r="75" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B75" s="10" t="s">
+      <c r="B75" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C75" s="10"/>
-    </row>
-    <row r="76" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C75" s="8"/>
+    </row>
+    <row r="76" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B76" s="10" t="s">
+      <c r="B76" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C76" s="10"/>
-    </row>
-    <row r="77" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C76" s="8"/>
+    </row>
+    <row r="77" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B77" s="10" t="s">
+      <c r="B77" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C77" s="10"/>
-    </row>
-    <row r="78" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C77" s="8"/>
+    </row>
+    <row r="78" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B78" s="10" t="s">
+      <c r="B78" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C78" s="10"/>
-    </row>
-    <row r="79" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C78" s="8"/>
+    </row>
+    <row r="79" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B79" s="10" t="s">
+      <c r="B79" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C79" s="10"/>
-    </row>
-    <row r="80" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C79" s="8"/>
+    </row>
+    <row r="80" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B80" s="10" t="s">
+      <c r="B80" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="C80" s="10"/>
-    </row>
-    <row r="81" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C80" s="8"/>
+    </row>
+    <row r="81" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B81" s="10" t="s">
+      <c r="B81" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C81" s="10"/>
-    </row>
-    <row r="82" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C81" s="8"/>
+    </row>
+    <row r="82" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B82" s="10" t="s">
+      <c r="B82" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C82" s="10"/>
-    </row>
-    <row r="83" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C82" s="8"/>
+    </row>
+    <row r="83" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B83" s="10" t="s">
+      <c r="B83" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="C83" s="10"/>
-    </row>
-    <row r="84" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C83" s="8"/>
+    </row>
+    <row r="84" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B84" s="10" t="s">
+      <c r="B84" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C84" s="10"/>
-    </row>
-    <row r="85" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C84" s="8"/>
+    </row>
+    <row r="85" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B85" s="10" t="s">
+      <c r="B85" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="C85" s="10"/>
-    </row>
-    <row r="86" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C85" s="8"/>
+    </row>
+    <row r="86" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B86" s="10" t="s">
+      <c r="B86" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="C86" s="10"/>
-    </row>
-    <row r="87" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C86" s="8"/>
+    </row>
+    <row r="87" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B87" s="10" t="s">
+      <c r="B87" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C87" s="10"/>
-    </row>
-    <row r="88" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C87" s="8"/>
+    </row>
+    <row r="88" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B88" s="10" t="s">
+      <c r="B88" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C88" s="10"/>
-    </row>
-    <row r="89" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C88" s="8"/>
+    </row>
+    <row r="89" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B89" s="10" t="s">
+      <c r="B89" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C89" s="10"/>
-    </row>
-    <row r="90" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C89" s="8"/>
+    </row>
+    <row r="90" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B90" s="10" t="s">
+      <c r="B90" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="C90" s="10"/>
-    </row>
-    <row r="91" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C90" s="8"/>
+    </row>
+    <row r="91" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B91" s="10" t="s">
+      <c r="B91" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C91" s="10"/>
-    </row>
-    <row r="92" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C91" s="8"/>
+    </row>
+    <row r="92" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B92" s="10" t="s">
+      <c r="B92" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="C92" s="10"/>
-    </row>
-    <row r="93" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C92" s="8"/>
+    </row>
+    <row r="93" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B93" s="10" t="s">
+      <c r="B93" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C93" s="10"/>
-    </row>
-    <row r="94" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C93" s="8"/>
+    </row>
+    <row r="94" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B94" s="10" t="s">
+      <c r="B94" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="C94" s="10"/>
-    </row>
-    <row r="95" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C94" s="8"/>
+    </row>
+    <row r="95" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B95" s="10" t="s">
+      <c r="B95" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="C95" s="10"/>
-    </row>
-    <row r="96" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C95" s="8"/>
+    </row>
+    <row r="96" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B96" s="10" t="s">
+      <c r="B96" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="C96" s="10"/>
-    </row>
-    <row r="97" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C96" s="8"/>
+    </row>
+    <row r="97" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B97" s="10" t="s">
+      <c r="B97" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C97" s="10"/>
-    </row>
-    <row r="98" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C97" s="8"/>
+    </row>
+    <row r="98" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B98" s="10" t="s">
+      <c r="B98" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="C98" s="10"/>
-    </row>
-    <row r="99" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C98" s="8"/>
+    </row>
+    <row r="99" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B99" s="10" t="s">
+      <c r="B99" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="C99" s="10"/>
-    </row>
-    <row r="100" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C99" s="8"/>
+    </row>
+    <row r="100" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B100" s="10" t="s">
+      <c r="B100" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C100" s="10"/>
-    </row>
-    <row r="101" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C100" s="8"/>
+    </row>
+    <row r="101" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B101" s="10" t="s">
+      <c r="B101" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="C101" s="10"/>
-    </row>
-    <row r="102" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C101" s="8"/>
+    </row>
+    <row r="102" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B102" s="10" t="s">
+      <c r="B102" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="C102" s="10"/>
-    </row>
-    <row r="103" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C102" s="8"/>
+    </row>
+    <row r="103" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B103" s="10" t="s">
+      <c r="B103" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="C103" s="10"/>
-    </row>
-    <row r="104" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C103" s="8"/>
+    </row>
+    <row r="104" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B104" s="10" t="s">
+      <c r="B104" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="C104" s="10"/>
-    </row>
-    <row r="105" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C104" s="8"/>
+    </row>
+    <row r="105" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B105" s="10" t="s">
+      <c r="B105" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="C105" s="10"/>
-    </row>
-    <row r="106" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C105" s="8"/>
+    </row>
+    <row r="106" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B106" s="10" t="s">
+      <c r="B106" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="C106" s="10"/>
-    </row>
-    <row r="107" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C106" s="8"/>
+    </row>
+    <row r="107" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B107" s="10" t="s">
+      <c r="B107" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="C107" s="10"/>
-    </row>
-    <row r="108" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C107" s="8"/>
+    </row>
+    <row r="108" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B108" s="10" t="s">
+      <c r="B108" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="C108" s="10"/>
-    </row>
-    <row r="109" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C108" s="8"/>
+    </row>
+    <row r="109" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B109" s="10" t="s">
+      <c r="B109" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="C109" s="10"/>
-    </row>
-    <row r="110" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C109" s="8"/>
+    </row>
+    <row r="110" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B110" s="10" t="s">
+      <c r="B110" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="C110" s="10"/>
-    </row>
-    <row r="111" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C110" s="8"/>
+    </row>
+    <row r="111" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B111" s="10" t="s">
+      <c r="B111" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="C111" s="10"/>
-    </row>
-    <row r="112" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C111" s="8"/>
+    </row>
+    <row r="112" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B112" s="10" t="s">
+      <c r="B112" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="C112" s="10"/>
-    </row>
-    <row r="113" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C112" s="8"/>
+    </row>
+    <row r="113" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B113" s="10" t="s">
+      <c r="B113" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="C113" s="10"/>
-    </row>
-    <row r="114" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C113" s="8"/>
+    </row>
+    <row r="114" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B114" s="10" t="s">
+      <c r="B114" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="C114" s="10"/>
-    </row>
-    <row r="115" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C114" s="8"/>
+    </row>
+    <row r="115" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B115" s="10" t="s">
+      <c r="B115" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="C115" s="10"/>
-    </row>
-    <row r="116" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C115" s="8"/>
+    </row>
+    <row r="116" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B116" s="10" t="s">
+      <c r="B116" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="C116" s="10"/>
-    </row>
-    <row r="117" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C116" s="8"/>
+    </row>
+    <row r="117" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B117" s="10" t="s">
+      <c r="B117" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="C117" s="10"/>
-    </row>
-    <row r="118" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C117" s="8"/>
+    </row>
+    <row r="118" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B118" s="10" t="s">
+      <c r="B118" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="C118" s="10"/>
-    </row>
-    <row r="119" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C118" s="8"/>
+    </row>
+    <row r="119" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B119" s="10" t="s">
+      <c r="B119" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="C119" s="10"/>
-    </row>
-    <row r="120" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C119" s="8"/>
+    </row>
+    <row r="120" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B120" s="10" t="s">
+      <c r="B120" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="C120" s="10"/>
-    </row>
-    <row r="121" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C120" s="8"/>
+    </row>
+    <row r="121" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B121" s="10" t="s">
+      <c r="B121" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="C121" s="10"/>
-    </row>
-    <row r="122" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C121" s="8"/>
+    </row>
+    <row r="122" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B122" s="10" t="s">
+      <c r="B122" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="C122" s="10"/>
-    </row>
-    <row r="123" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C122" s="8"/>
+    </row>
+    <row r="123" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B123" s="10" t="s">
+      <c r="B123" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="C123" s="10"/>
-    </row>
-    <row r="124" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C123" s="8"/>
+    </row>
+    <row r="124" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B124" s="10" t="s">
+      <c r="B124" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="C124" s="10"/>
-    </row>
-    <row r="125" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C124" s="8"/>
+    </row>
+    <row r="125" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B125" s="10" t="s">
+      <c r="B125" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="C125" s="10"/>
-    </row>
-    <row r="126" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C125" s="8"/>
+    </row>
+    <row r="126" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B126" s="10" t="s">
+      <c r="B126" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="C126" s="10"/>
-    </row>
-    <row r="127" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C126" s="8"/>
+    </row>
+    <row r="127" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B127" s="10" t="s">
+      <c r="B127" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="C127" s="10"/>
-    </row>
-    <row r="128" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C127" s="8"/>
+    </row>
+    <row r="128" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B128" s="10" t="s">
+      <c r="B128" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="C128" s="10"/>
-    </row>
-    <row r="129" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C128" s="8"/>
+    </row>
+    <row r="129" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B129" s="10" t="s">
+      <c r="B129" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="C129" s="10"/>
-    </row>
-    <row r="130" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C129" s="8"/>
+    </row>
+    <row r="130" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B130" s="10" t="s">
+      <c r="B130" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="C130" s="10"/>
-    </row>
-    <row r="131" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C130" s="8"/>
+    </row>
+    <row r="131" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B131" s="10" t="s">
+      <c r="B131" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="C131" s="10"/>
-    </row>
-    <row r="132" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C131" s="8"/>
+    </row>
+    <row r="132" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B132" s="10" t="s">
+      <c r="B132" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="C132" s="10"/>
-    </row>
-    <row r="133" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C132" s="8"/>
+    </row>
+    <row r="133" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B133" s="10" t="s">
+      <c r="B133" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="C133" s="10"/>
-    </row>
-    <row r="134" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C133" s="8"/>
+    </row>
+    <row r="134" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B134" s="10" t="s">
+      <c r="B134" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="C134" s="10"/>
-    </row>
-    <row r="135" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C134" s="8"/>
+    </row>
+    <row r="135" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B135" s="10" t="s">
+      <c r="B135" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="C135" s="10"/>
-    </row>
-    <row r="136" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C135" s="8"/>
+    </row>
+    <row r="136" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B136" s="10" t="s">
+      <c r="B136" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="C136" s="10"/>
-    </row>
-    <row r="137" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C136" s="8"/>
+    </row>
+    <row r="137" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B137" s="10" t="s">
+      <c r="B137" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="C137" s="10"/>
-    </row>
-    <row r="138" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C137" s="8"/>
+    </row>
+    <row r="138" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B138" s="10" t="s">
+      <c r="B138" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="C138" s="10"/>
-    </row>
-    <row r="139" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C138" s="8"/>
+    </row>
+    <row r="139" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B139" s="10" t="s">
+      <c r="B139" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="C139" s="10"/>
-    </row>
-    <row r="140" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C139" s="8"/>
+    </row>
+    <row r="140" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B140" s="10" t="s">
+      <c r="B140" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="C140" s="10"/>
-    </row>
-    <row r="141" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C140" s="8"/>
+    </row>
+    <row r="141" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B141" s="10" t="s">
+      <c r="B141" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="C141" s="10"/>
-    </row>
-    <row r="142" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C141" s="8"/>
+    </row>
+    <row r="142" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B142" s="10" t="s">
+      <c r="B142" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="C142" s="10"/>
-    </row>
-    <row r="143" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C142" s="8"/>
+    </row>
+    <row r="143" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B143" s="10" t="s">
+      <c r="B143" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="C143" s="10"/>
-    </row>
-    <row r="144" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C143" s="8"/>
+    </row>
+    <row r="144" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B144" s="10" t="s">
+      <c r="B144" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="C144" s="10"/>
-    </row>
-    <row r="145" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C144" s="8"/>
+    </row>
+    <row r="145" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B145" s="10" t="s">
+      <c r="B145" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="C145" s="10"/>
-    </row>
-    <row r="146" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C145" s="8"/>
+    </row>
+    <row r="146" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B146" s="10" t="s">
+      <c r="B146" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="C146" s="10"/>
-    </row>
-    <row r="147" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C146" s="8"/>
+    </row>
+    <row r="147" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B147" s="10" t="s">
+      <c r="B147" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="C147" s="10"/>
-    </row>
-    <row r="148" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C147" s="8"/>
+    </row>
+    <row r="148" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B148" s="10" t="s">
+      <c r="B148" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="C148" s="10"/>
-    </row>
-    <row r="149" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C148" s="8"/>
+    </row>
+    <row r="149" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B149" s="10" t="s">
+      <c r="B149" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="C149" s="10"/>
-    </row>
-    <row r="150" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C149" s="8"/>
+    </row>
+    <row r="150" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B150" s="10" t="s">
+      <c r="B150" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="C150" s="10"/>
-    </row>
-    <row r="151" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C150" s="8"/>
+    </row>
+    <row r="151" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B151" s="10" t="s">
+      <c r="B151" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="C151" s="10"/>
-    </row>
-    <row r="152" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C151" s="8"/>
+    </row>
+    <row r="152" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B152" s="10" t="s">
+      <c r="B152" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="C152" s="10"/>
-    </row>
-    <row r="153" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C152" s="8"/>
+    </row>
+    <row r="153" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B153" s="10" t="s">
+      <c r="B153" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="C153" s="10"/>
-    </row>
-    <row r="154" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C153" s="8"/>
+    </row>
+    <row r="154" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B154" s="10" t="s">
+      <c r="B154" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="C154" s="10"/>
-    </row>
-    <row r="155" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C154" s="8"/>
+    </row>
+    <row r="155" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B155" s="10" t="s">
+      <c r="B155" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="C155" s="10"/>
-    </row>
-    <row r="156" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C155" s="8"/>
+    </row>
+    <row r="156" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B156" s="10" t="s">
+      <c r="B156" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="C156" s="10"/>
-    </row>
-    <row r="157" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C156" s="8"/>
+    </row>
+    <row r="157" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B157" s="10" t="s">
+      <c r="B157" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="C157" s="10"/>
-    </row>
-    <row r="158" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C157" s="8"/>
+    </row>
+    <row r="158" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B158" s="10" t="s">
+      <c r="B158" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="C158" s="10"/>
-    </row>
-    <row r="159" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C158" s="8"/>
+    </row>
+    <row r="159" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B159" s="10" t="s">
+      <c r="B159" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="C159" s="10"/>
-    </row>
-    <row r="160" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C159" s="8"/>
+    </row>
+    <row r="160" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B160" s="10" t="s">
+      <c r="B160" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="C160" s="10"/>
-    </row>
-    <row r="161" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C160" s="8"/>
+    </row>
+    <row r="161" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B161" s="10" t="s">
+      <c r="B161" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="C161" s="10"/>
-    </row>
-    <row r="162" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C161" s="8"/>
+    </row>
+    <row r="162" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B162" s="10" t="s">
+      <c r="B162" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="C162" s="10"/>
-    </row>
-    <row r="163" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C162" s="8"/>
+    </row>
+    <row r="163" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B163" s="10" t="s">
+      <c r="B163" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="C163" s="10"/>
-    </row>
-    <row r="164" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C163" s="8"/>
+    </row>
+    <row r="164" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B164" s="10" t="s">
+      <c r="B164" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="C164" s="10"/>
-    </row>
-    <row r="165" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C164" s="8"/>
+    </row>
+    <row r="165" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B165" s="10" t="s">
+      <c r="B165" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="C165" s="10"/>
-    </row>
-    <row r="166" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C165" s="8"/>
+    </row>
+    <row r="166" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B166" s="10" t="s">
+      <c r="B166" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="C166" s="10"/>
-    </row>
-    <row r="167" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C166" s="8"/>
+    </row>
+    <row r="167" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B167" s="10" t="s">
+      <c r="B167" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="C167" s="10"/>
-    </row>
-    <row r="168" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C167" s="8"/>
+    </row>
+    <row r="168" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B168" s="10" t="s">
+      <c r="B168" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="C168" s="10"/>
-    </row>
-    <row r="169" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C168" s="8"/>
+    </row>
+    <row r="169" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B169" s="10" t="s">
+      <c r="B169" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="C169" s="10"/>
-    </row>
-    <row r="170" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C169" s="8"/>
+    </row>
+    <row r="170" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B170" s="10" t="s">
+      <c r="B170" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="C170" s="10"/>
-    </row>
-    <row r="171" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C170" s="8"/>
+    </row>
+    <row r="171" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B171" s="10" t="s">
+      <c r="B171" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="C171" s="10"/>
-    </row>
-    <row r="172" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C171" s="8"/>
+    </row>
+    <row r="172" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B172" s="10" t="s">
+      <c r="B172" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="C172" s="10"/>
-    </row>
-    <row r="173" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C172" s="8"/>
+    </row>
+    <row r="173" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B173" s="10" t="s">
+      <c r="B173" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="C173" s="10"/>
-    </row>
-    <row r="174" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C173" s="8"/>
+    </row>
+    <row r="174" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B174" s="10" t="s">
+      <c r="B174" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="C174" s="10"/>
-    </row>
-    <row r="175" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C174" s="8"/>
+    </row>
+    <row r="175" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B175" s="10" t="s">
+      <c r="B175" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="C175" s="10"/>
-    </row>
-    <row r="176" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C175" s="8"/>
+    </row>
+    <row r="176" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B176" s="10" t="s">
+      <c r="B176" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="C176" s="10"/>
-    </row>
-    <row r="177" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C176" s="8"/>
+    </row>
+    <row r="177" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B177" s="10" t="s">
+      <c r="B177" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="C177" s="10"/>
-    </row>
-    <row r="178" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C177" s="8"/>
+    </row>
+    <row r="178" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B178" s="10" t="s">
+      <c r="B178" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="C178" s="10"/>
-    </row>
-    <row r="179" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C178" s="8"/>
+    </row>
+    <row r="179" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B179" s="10" t="s">
+      <c r="B179" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="C179" s="10"/>
-    </row>
-    <row r="180" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C179" s="8"/>
+    </row>
+    <row r="180" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B180" s="10" t="s">
+      <c r="B180" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="C180" s="10"/>
-    </row>
-    <row r="181" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C180" s="8"/>
+    </row>
+    <row r="181" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B181" s="10" t="s">
+      <c r="B181" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="C181" s="10"/>
-    </row>
-    <row r="182" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C181" s="8"/>
+    </row>
+    <row r="182" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B182" s="10" t="s">
+      <c r="B182" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="C182" s="10"/>
-    </row>
-    <row r="183" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C182" s="8"/>
+    </row>
+    <row r="183" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B183" s="10" t="s">
+      <c r="B183" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="C183" s="10"/>
-    </row>
-    <row r="184" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C183" s="8"/>
+    </row>
+    <row r="184" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B184" s="10" t="s">
+      <c r="B184" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="C184" s="10"/>
-    </row>
-    <row r="185" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C184" s="8"/>
+    </row>
+    <row r="185" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B185" s="10" t="s">
+      <c r="B185" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="C185" s="10"/>
-    </row>
-    <row r="186" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C185" s="8"/>
+    </row>
+    <row r="186" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B186" s="10" t="s">
+      <c r="B186" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="C186" s="10"/>
-    </row>
-    <row r="187" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C186" s="8"/>
+    </row>
+    <row r="187" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B187" s="10" t="s">
+      <c r="B187" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="C187" s="10"/>
-    </row>
-    <row r="188" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C187" s="8"/>
+    </row>
+    <row r="188" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B188" s="10" t="s">
+      <c r="B188" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="C188" s="10"/>
-    </row>
-    <row r="189" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C188" s="8"/>
+    </row>
+    <row r="189" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B189" s="10" t="s">
+      <c r="B189" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="C189" s="10"/>
-    </row>
-    <row r="190" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C189" s="8"/>
+    </row>
+    <row r="190" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B190" s="10" t="s">
+      <c r="B190" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="C190" s="10"/>
-    </row>
-    <row r="191" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C190" s="8"/>
+    </row>
+    <row r="191" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B191" s="10" t="s">
+      <c r="B191" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="C191" s="10"/>
-    </row>
-    <row r="192" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C191" s="8"/>
+    </row>
+    <row r="192" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B192" s="10" t="s">
+      <c r="B192" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="C192" s="10"/>
-    </row>
-    <row r="193" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C192" s="8"/>
+    </row>
+    <row r="193" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B193" s="10" t="s">
+      <c r="B193" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="C193" s="10"/>
-    </row>
-    <row r="194" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C193" s="8"/>
+    </row>
+    <row r="194" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B194" s="10" t="s">
+      <c r="B194" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="C194" s="10"/>
-    </row>
-    <row r="195" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C194" s="8"/>
+    </row>
+    <row r="195" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B195" s="10" t="s">
+      <c r="B195" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="C195" s="10"/>
-    </row>
-    <row r="196" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C195" s="8"/>
+    </row>
+    <row r="196" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B196" s="10" t="s">
+      <c r="B196" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="C196" s="10"/>
-    </row>
-    <row r="197" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C196" s="8"/>
+    </row>
+    <row r="197" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A197" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B197" s="10" t="s">
+      <c r="B197" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="C197" s="10"/>
-    </row>
-    <row r="198" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C197" s="8"/>
+    </row>
+    <row r="198" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A198" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B198" s="10" t="s">
+      <c r="B198" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="C198" s="10"/>
-    </row>
-    <row r="199" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C198" s="8"/>
+    </row>
+    <row r="199" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A199" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B199" s="10" t="s">
+      <c r="B199" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="C199" s="10"/>
-    </row>
-    <row r="200" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C199" s="8"/>
+    </row>
+    <row r="200" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A200" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B200" s="10" t="s">
+      <c r="B200" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="C200" s="10"/>
-    </row>
-    <row r="201" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C200" s="8"/>
+    </row>
+    <row r="201" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A201" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B201" s="10" t="s">
+      <c r="B201" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="C201" s="10"/>
-    </row>
-    <row r="202" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C201" s="8"/>
+    </row>
+    <row r="202" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A202" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B202" s="10" t="s">
+      <c r="B202" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="C202" s="10"/>
-    </row>
-    <row r="203" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C202" s="8"/>
+    </row>
+    <row r="203" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A203" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B203" s="10" t="s">
+      <c r="B203" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="C203" s="10"/>
-    </row>
-    <row r="204" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C203" s="8"/>
+    </row>
+    <row r="204" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B204" s="10" t="s">
+      <c r="B204" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="C204" s="10"/>
-    </row>
-    <row r="205" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C204" s="8"/>
+    </row>
+    <row r="205" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B205" s="10" t="s">
+      <c r="B205" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="C205" s="10"/>
-    </row>
-    <row r="206" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C205" s="8"/>
+    </row>
+    <row r="206" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B206" s="10" t="s">
+      <c r="B206" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="C206" s="10"/>
-    </row>
-    <row r="207" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C206" s="8"/>
+    </row>
+    <row r="207" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B207" s="10" t="s">
+      <c r="B207" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="C207" s="10"/>
-    </row>
-    <row r="208" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C207" s="8"/>
+    </row>
+    <row r="208" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B208" s="10" t="s">
+      <c r="B208" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="C208" s="10"/>
-    </row>
-    <row r="209" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C208" s="8"/>
+    </row>
+    <row r="209" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A209" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B209" s="10" t="s">
+      <c r="B209" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="C209" s="10"/>
-    </row>
-    <row r="210" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C209" s="8"/>
+    </row>
+    <row r="210" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A210" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B210" s="10" t="s">
+      <c r="B210" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="C210" s="10"/>
-    </row>
-    <row r="211" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C210" s="8"/>
+    </row>
+    <row r="211" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A211" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B211" s="10" t="s">
+      <c r="B211" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="C211" s="10"/>
-    </row>
-    <row r="212" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C211" s="8"/>
+    </row>
+    <row r="212" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B212" s="10" t="s">
+      <c r="B212" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="C212" s="10"/>
-    </row>
-    <row r="213" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C212" s="8"/>
+    </row>
+    <row r="213" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A213" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B213" s="10" t="s">
+      <c r="B213" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="C213" s="10"/>
-    </row>
-    <row r="214" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C213" s="8"/>
+    </row>
+    <row r="214" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A214" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B214" s="10" t="s">
+      <c r="B214" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="C214" s="10"/>
-    </row>
-    <row r="215" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C214" s="8"/>
+    </row>
+    <row r="215" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A215" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B215" s="10" t="s">
+      <c r="B215" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="C215" s="10"/>
-    </row>
-    <row r="216" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C215" s="8"/>
+    </row>
+    <row r="216" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A216" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B216" s="10" t="s">
+      <c r="B216" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="C216" s="10"/>
-    </row>
-    <row r="217" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C216" s="8"/>
+    </row>
+    <row r="217" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A217" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B217" s="10" t="s">
+      <c r="B217" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="C217" s="10"/>
-    </row>
-    <row r="218" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C217" s="8"/>
+    </row>
+    <row r="218" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A218" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B218" s="10" t="s">
+      <c r="B218" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="C218" s="10"/>
-    </row>
-    <row r="219" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C218" s="8"/>
+    </row>
+    <row r="219" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A219" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B219" s="10" t="s">
+      <c r="B219" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="C219" s="10"/>
-    </row>
-    <row r="220" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C219" s="8"/>
+    </row>
+    <row r="220" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A220" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B220" s="10" t="s">
+      <c r="B220" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="C220" s="10"/>
-    </row>
-    <row r="221" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C220" s="8"/>
+    </row>
+    <row r="221" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A221" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B221" s="10" t="s">
+      <c r="B221" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="C221" s="10"/>
-    </row>
-    <row r="222" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C221" s="8"/>
+    </row>
+    <row r="222" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B222" s="10" t="s">
+      <c r="B222" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="C222" s="10"/>
-    </row>
-    <row r="223" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C222" s="8"/>
+    </row>
+    <row r="223" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A223" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B223" s="10" t="s">
+      <c r="B223" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="C223" s="10"/>
-    </row>
-    <row r="224" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C223" s="8"/>
+    </row>
+    <row r="224" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B224" s="10" t="s">
+      <c r="B224" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="C224" s="10"/>
-    </row>
-    <row r="225" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C224" s="8"/>
+    </row>
+    <row r="225" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A225" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B225" s="10" t="s">
+      <c r="B225" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="C225" s="10"/>
-    </row>
-    <row r="226" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C225" s="8"/>
+    </row>
+    <row r="226" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B226" s="10" t="s">
+      <c r="B226" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="C226" s="10"/>
-    </row>
-    <row r="227" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C226" s="8"/>
+    </row>
+    <row r="227" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B227" s="10" t="s">
+      <c r="B227" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="C227" s="10"/>
-    </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A228" s="10"/>
-      <c r="B228" s="10"/>
-      <c r="C228" s="10"/>
-    </row>
-    <row r="229" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C227" s="8"/>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A228" s="8"/>
+      <c r="B228" s="8"/>
+      <c r="C228" s="8"/>
+    </row>
+    <row r="229" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A229" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="B229" s="10" t="s">
+      <c r="B229" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C229" s="10"/>
-    </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A230" s="10"/>
-      <c r="B230" s="10"/>
-      <c r="C230" s="10"/>
-    </row>
-    <row r="231" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C229" s="8"/>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A230" s="8"/>
+      <c r="B230" s="8"/>
+      <c r="C230" s="8"/>
+    </row>
+    <row r="231" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A231" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="B231" s="10" t="s">
+      <c r="B231" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C231" s="10"/>
-    </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A232" s="10"/>
-      <c r="B232" s="10"/>
-      <c r="C232" s="10"/>
-    </row>
-    <row r="233" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C231" s="8"/>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A232" s="8"/>
+      <c r="B232" s="8"/>
+      <c r="C232" s="8"/>
+    </row>
+    <row r="233" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A233" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="B233" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C233" s="10"/>
-    </row>
-    <row r="234" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B233" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C233" s="8"/>
+    </row>
+    <row r="234" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A234" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="B234" s="10" t="s">
+      <c r="B234" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C234" s="10"/>
-    </row>
-    <row r="235" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C234" s="8"/>
+    </row>
+    <row r="235" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A235" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B235" s="10" t="s">
+      <c r="B235" s="8" t="s">
         <v>239</v>
       </c>
-      <c r="C235" s="10"/>
-    </row>
-    <row r="236" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C235" s="8"/>
+    </row>
+    <row r="236" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A236" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="B236" s="10" t="s">
+      <c r="B236" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C236" s="10"/>
-    </row>
-    <row r="237" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C236" s="8"/>
+    </row>
+    <row r="237" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A237" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="B237" s="10" t="s">
+      <c r="B237" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C237" s="10"/>
-    </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A238" s="10"/>
-      <c r="B238" s="10"/>
-      <c r="C238" s="10"/>
-    </row>
-    <row r="239" spans="1:3" ht="25.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C237" s="8"/>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A238" s="8"/>
+      <c r="B238" s="8"/>
+      <c r="C238" s="8"/>
+    </row>
+    <row r="239" spans="1:3" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A239" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="B239" s="10" t="s">
+      <c r="B239" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="C239" s="10"/>
-    </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A240" s="10"/>
-      <c r="B240" s="10"/>
-      <c r="C240" s="10"/>
-    </row>
-    <row r="241" spans="1:3" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C239" s="8"/>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A240" s="8"/>
+      <c r="B240" s="8"/>
+      <c r="C240" s="8"/>
+    </row>
+    <row r="241" spans="1:3" ht="64.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A241" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="B241" s="10" t="s">
+      <c r="B241" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="C241" s="10"/>
-    </row>
-    <row r="242" spans="1:3" ht="89.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C241" s="8"/>
+    </row>
+    <row r="242" spans="1:3" ht="89.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A242" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B242" s="10" t="s">
+      <c r="B242" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="C242" s="10"/>
-    </row>
-    <row r="243" spans="1:3" ht="25.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C242" s="8"/>
+    </row>
+    <row r="243" spans="1:3" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A243" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B243" s="10" t="s">
+      <c r="B243" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="C243" s="10"/>
-    </row>
-    <row r="244" spans="1:3" ht="89.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C243" s="8"/>
+    </row>
+    <row r="244" spans="1:3" ht="89.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A244" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B244" s="10" t="s">
+      <c r="B244" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="C244" s="10"/>
-    </row>
-    <row r="245" spans="1:3" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C244" s="8"/>
+    </row>
+    <row r="245" spans="1:3" ht="64.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A245" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B245" s="10" t="s">
+      <c r="B245" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="C245" s="10"/>
-    </row>
-    <row r="246" spans="1:3" ht="51.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C245" s="8"/>
+    </row>
+    <row r="246" spans="1:3" ht="51.3" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A246" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B246" s="10" t="s">
+      <c r="B246" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="C246" s="10"/>
-    </row>
-    <row r="247" spans="1:3" ht="25.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C246" s="8"/>
+    </row>
+    <row r="247" spans="1:3" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A247" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B247" s="10" t="s">
+      <c r="B247" s="8" t="s">
         <v>251</v>
       </c>
-      <c r="C247" s="10"/>
-    </row>
-    <row r="248" spans="1:3" ht="51.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C247" s="8"/>
+    </row>
+    <row r="248" spans="1:3" ht="51.3" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A248" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B248" s="10" t="s">
+      <c r="B248" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="C248" s="10"/>
-    </row>
-    <row r="249" spans="1:3" ht="38.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C248" s="8"/>
+    </row>
+    <row r="249" spans="1:3" ht="38.549999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A249" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B249" s="10" t="s">
+      <c r="B249" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="C249" s="10"/>
-    </row>
-    <row r="250" spans="1:3" ht="140.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C249" s="8"/>
+    </row>
+    <row r="250" spans="1:3" ht="140.69999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A250" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B250" s="10" t="s">
+      <c r="B250" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="C250" s="10"/>
-    </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A251" s="10"/>
-      <c r="B251" s="10"/>
-      <c r="C251" s="10"/>
-    </row>
-    <row r="252" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C250" s="8"/>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A251" s="8"/>
+      <c r="B251" s="8"/>
+      <c r="C251" s="8"/>
+    </row>
+    <row r="252" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A252" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="B252" s="10" t="s">
+      <c r="B252" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C252" s="10"/>
-    </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A253" s="10"/>
-      <c r="B253" s="10"/>
-      <c r="C253" s="10"/>
+      <c r="C252" s="8"/>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A253" s="8"/>
+      <c r="B253" s="8"/>
+      <c r="C253" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="253">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="B93:C93"/>
-    <mergeCell ref="B94:C94"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="B97:C97"/>
-    <mergeCell ref="B98:C98"/>
-    <mergeCell ref="B99:C99"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="B101:C101"/>
-    <mergeCell ref="B102:C102"/>
-    <mergeCell ref="B103:C103"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="B109:C109"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="B111:C111"/>
-    <mergeCell ref="B112:C112"/>
-    <mergeCell ref="B113:C113"/>
-    <mergeCell ref="B114:C114"/>
-    <mergeCell ref="B115:C115"/>
-    <mergeCell ref="B116:C116"/>
-    <mergeCell ref="B117:C117"/>
-    <mergeCell ref="B118:C118"/>
-    <mergeCell ref="B119:C119"/>
-    <mergeCell ref="B120:C120"/>
-    <mergeCell ref="B121:C121"/>
-    <mergeCell ref="B122:C122"/>
-    <mergeCell ref="B123:C123"/>
-    <mergeCell ref="B124:C124"/>
-    <mergeCell ref="B125:C125"/>
-    <mergeCell ref="B126:C126"/>
-    <mergeCell ref="B127:C127"/>
-    <mergeCell ref="B128:C128"/>
-    <mergeCell ref="B129:C129"/>
-    <mergeCell ref="B130:C130"/>
-    <mergeCell ref="B131:C131"/>
-    <mergeCell ref="B132:C132"/>
-    <mergeCell ref="B133:C133"/>
-    <mergeCell ref="B134:C134"/>
-    <mergeCell ref="B135:C135"/>
-    <mergeCell ref="B136:C136"/>
-    <mergeCell ref="B137:C137"/>
-    <mergeCell ref="B138:C138"/>
-    <mergeCell ref="B139:C139"/>
-    <mergeCell ref="B140:C140"/>
-    <mergeCell ref="B141:C141"/>
-    <mergeCell ref="B142:C142"/>
-    <mergeCell ref="B143:C143"/>
-    <mergeCell ref="B144:C144"/>
-    <mergeCell ref="B145:C145"/>
-    <mergeCell ref="B146:C146"/>
-    <mergeCell ref="B147:C147"/>
-    <mergeCell ref="B148:C148"/>
-    <mergeCell ref="B149:C149"/>
-    <mergeCell ref="B150:C150"/>
-    <mergeCell ref="B151:C151"/>
-    <mergeCell ref="B152:C152"/>
-    <mergeCell ref="B153:C153"/>
-    <mergeCell ref="B154:C154"/>
-    <mergeCell ref="B155:C155"/>
-    <mergeCell ref="B156:C156"/>
-    <mergeCell ref="B157:C157"/>
-    <mergeCell ref="B158:C158"/>
-    <mergeCell ref="B159:C159"/>
-    <mergeCell ref="B160:C160"/>
-    <mergeCell ref="B161:C161"/>
-    <mergeCell ref="B162:C162"/>
-    <mergeCell ref="B163:C163"/>
-    <mergeCell ref="B164:C164"/>
-    <mergeCell ref="B165:C165"/>
-    <mergeCell ref="B166:C166"/>
-    <mergeCell ref="B167:C167"/>
-    <mergeCell ref="B168:C168"/>
-    <mergeCell ref="B169:C169"/>
-    <mergeCell ref="B170:C170"/>
-    <mergeCell ref="B171:C171"/>
-    <mergeCell ref="B172:C172"/>
-    <mergeCell ref="B173:C173"/>
-    <mergeCell ref="B174:C174"/>
-    <mergeCell ref="B175:C175"/>
-    <mergeCell ref="B176:C176"/>
-    <mergeCell ref="B177:C177"/>
-    <mergeCell ref="B178:C178"/>
-    <mergeCell ref="B179:C179"/>
-    <mergeCell ref="B180:C180"/>
-    <mergeCell ref="B181:C181"/>
-    <mergeCell ref="B182:C182"/>
-    <mergeCell ref="B183:C183"/>
-    <mergeCell ref="B184:C184"/>
-    <mergeCell ref="B185:C185"/>
-    <mergeCell ref="B186:C186"/>
-    <mergeCell ref="B187:C187"/>
-    <mergeCell ref="B188:C188"/>
-    <mergeCell ref="B189:C189"/>
-    <mergeCell ref="B190:C190"/>
-    <mergeCell ref="B191:C191"/>
-    <mergeCell ref="B192:C192"/>
-    <mergeCell ref="B193:C193"/>
-    <mergeCell ref="B194:C194"/>
-    <mergeCell ref="B195:C195"/>
-    <mergeCell ref="B196:C196"/>
-    <mergeCell ref="B197:C197"/>
-    <mergeCell ref="B198:C198"/>
-    <mergeCell ref="B199:C199"/>
-    <mergeCell ref="B200:C200"/>
-    <mergeCell ref="B201:C201"/>
-    <mergeCell ref="B202:C202"/>
-    <mergeCell ref="B203:C203"/>
-    <mergeCell ref="B204:C204"/>
-    <mergeCell ref="B205:C205"/>
-    <mergeCell ref="B206:C206"/>
-    <mergeCell ref="B207:C207"/>
-    <mergeCell ref="B208:C208"/>
-    <mergeCell ref="B209:C209"/>
-    <mergeCell ref="B210:C210"/>
-    <mergeCell ref="B211:C211"/>
-    <mergeCell ref="B212:C212"/>
-    <mergeCell ref="B213:C213"/>
-    <mergeCell ref="B214:C214"/>
-    <mergeCell ref="B215:C215"/>
-    <mergeCell ref="B216:C216"/>
-    <mergeCell ref="B217:C217"/>
-    <mergeCell ref="B218:C218"/>
-    <mergeCell ref="B219:C219"/>
-    <mergeCell ref="B220:C220"/>
-    <mergeCell ref="B221:C221"/>
-    <mergeCell ref="B222:C222"/>
-    <mergeCell ref="B223:C223"/>
-    <mergeCell ref="B224:C224"/>
-    <mergeCell ref="B225:C225"/>
-    <mergeCell ref="B226:C226"/>
-    <mergeCell ref="B227:C227"/>
-    <mergeCell ref="A228:C228"/>
-    <mergeCell ref="B229:C229"/>
-    <mergeCell ref="A230:C230"/>
-    <mergeCell ref="B231:C231"/>
-    <mergeCell ref="A232:C232"/>
-    <mergeCell ref="B233:C233"/>
-    <mergeCell ref="B234:C234"/>
-    <mergeCell ref="B235:C235"/>
-    <mergeCell ref="B236:C236"/>
-    <mergeCell ref="B237:C237"/>
-    <mergeCell ref="A238:C238"/>
-    <mergeCell ref="B239:C239"/>
-    <mergeCell ref="A240:C240"/>
-    <mergeCell ref="B241:C241"/>
-    <mergeCell ref="B242:C242"/>
-    <mergeCell ref="B243:C243"/>
     <mergeCell ref="A253:C253"/>
     <mergeCell ref="B244:C244"/>
     <mergeCell ref="B245:C245"/>
@@ -5068,6 +4819,249 @@
     <mergeCell ref="B250:C250"/>
     <mergeCell ref="A251:C251"/>
     <mergeCell ref="B252:C252"/>
+    <mergeCell ref="B235:C235"/>
+    <mergeCell ref="B236:C236"/>
+    <mergeCell ref="B237:C237"/>
+    <mergeCell ref="A238:C238"/>
+    <mergeCell ref="B239:C239"/>
+    <mergeCell ref="A240:C240"/>
+    <mergeCell ref="B241:C241"/>
+    <mergeCell ref="B242:C242"/>
+    <mergeCell ref="B243:C243"/>
+    <mergeCell ref="B226:C226"/>
+    <mergeCell ref="B227:C227"/>
+    <mergeCell ref="A228:C228"/>
+    <mergeCell ref="B229:C229"/>
+    <mergeCell ref="A230:C230"/>
+    <mergeCell ref="B231:C231"/>
+    <mergeCell ref="A232:C232"/>
+    <mergeCell ref="B233:C233"/>
+    <mergeCell ref="B234:C234"/>
+    <mergeCell ref="B217:C217"/>
+    <mergeCell ref="B218:C218"/>
+    <mergeCell ref="B219:C219"/>
+    <mergeCell ref="B220:C220"/>
+    <mergeCell ref="B221:C221"/>
+    <mergeCell ref="B222:C222"/>
+    <mergeCell ref="B223:C223"/>
+    <mergeCell ref="B224:C224"/>
+    <mergeCell ref="B225:C225"/>
+    <mergeCell ref="B208:C208"/>
+    <mergeCell ref="B209:C209"/>
+    <mergeCell ref="B210:C210"/>
+    <mergeCell ref="B211:C211"/>
+    <mergeCell ref="B212:C212"/>
+    <mergeCell ref="B213:C213"/>
+    <mergeCell ref="B214:C214"/>
+    <mergeCell ref="B215:C215"/>
+    <mergeCell ref="B216:C216"/>
+    <mergeCell ref="B199:C199"/>
+    <mergeCell ref="B200:C200"/>
+    <mergeCell ref="B201:C201"/>
+    <mergeCell ref="B202:C202"/>
+    <mergeCell ref="B203:C203"/>
+    <mergeCell ref="B204:C204"/>
+    <mergeCell ref="B205:C205"/>
+    <mergeCell ref="B206:C206"/>
+    <mergeCell ref="B207:C207"/>
+    <mergeCell ref="B190:C190"/>
+    <mergeCell ref="B191:C191"/>
+    <mergeCell ref="B192:C192"/>
+    <mergeCell ref="B193:C193"/>
+    <mergeCell ref="B194:C194"/>
+    <mergeCell ref="B195:C195"/>
+    <mergeCell ref="B196:C196"/>
+    <mergeCell ref="B197:C197"/>
+    <mergeCell ref="B198:C198"/>
+    <mergeCell ref="B181:C181"/>
+    <mergeCell ref="B182:C182"/>
+    <mergeCell ref="B183:C183"/>
+    <mergeCell ref="B184:C184"/>
+    <mergeCell ref="B185:C185"/>
+    <mergeCell ref="B186:C186"/>
+    <mergeCell ref="B187:C187"/>
+    <mergeCell ref="B188:C188"/>
+    <mergeCell ref="B189:C189"/>
+    <mergeCell ref="B172:C172"/>
+    <mergeCell ref="B173:C173"/>
+    <mergeCell ref="B174:C174"/>
+    <mergeCell ref="B175:C175"/>
+    <mergeCell ref="B176:C176"/>
+    <mergeCell ref="B177:C177"/>
+    <mergeCell ref="B178:C178"/>
+    <mergeCell ref="B179:C179"/>
+    <mergeCell ref="B180:C180"/>
+    <mergeCell ref="B163:C163"/>
+    <mergeCell ref="B164:C164"/>
+    <mergeCell ref="B165:C165"/>
+    <mergeCell ref="B166:C166"/>
+    <mergeCell ref="B167:C167"/>
+    <mergeCell ref="B168:C168"/>
+    <mergeCell ref="B169:C169"/>
+    <mergeCell ref="B170:C170"/>
+    <mergeCell ref="B171:C171"/>
+    <mergeCell ref="B154:C154"/>
+    <mergeCell ref="B155:C155"/>
+    <mergeCell ref="B156:C156"/>
+    <mergeCell ref="B157:C157"/>
+    <mergeCell ref="B158:C158"/>
+    <mergeCell ref="B159:C159"/>
+    <mergeCell ref="B160:C160"/>
+    <mergeCell ref="B161:C161"/>
+    <mergeCell ref="B162:C162"/>
+    <mergeCell ref="B145:C145"/>
+    <mergeCell ref="B146:C146"/>
+    <mergeCell ref="B147:C147"/>
+    <mergeCell ref="B148:C148"/>
+    <mergeCell ref="B149:C149"/>
+    <mergeCell ref="B150:C150"/>
+    <mergeCell ref="B151:C151"/>
+    <mergeCell ref="B152:C152"/>
+    <mergeCell ref="B153:C153"/>
+    <mergeCell ref="B136:C136"/>
+    <mergeCell ref="B137:C137"/>
+    <mergeCell ref="B138:C138"/>
+    <mergeCell ref="B139:C139"/>
+    <mergeCell ref="B140:C140"/>
+    <mergeCell ref="B141:C141"/>
+    <mergeCell ref="B142:C142"/>
+    <mergeCell ref="B143:C143"/>
+    <mergeCell ref="B144:C144"/>
+    <mergeCell ref="B127:C127"/>
+    <mergeCell ref="B128:C128"/>
+    <mergeCell ref="B129:C129"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="B131:C131"/>
+    <mergeCell ref="B132:C132"/>
+    <mergeCell ref="B133:C133"/>
+    <mergeCell ref="B134:C134"/>
+    <mergeCell ref="B135:C135"/>
+    <mergeCell ref="B118:C118"/>
+    <mergeCell ref="B119:C119"/>
+    <mergeCell ref="B120:C120"/>
+    <mergeCell ref="B121:C121"/>
+    <mergeCell ref="B122:C122"/>
+    <mergeCell ref="B123:C123"/>
+    <mergeCell ref="B124:C124"/>
+    <mergeCell ref="B125:C125"/>
+    <mergeCell ref="B126:C126"/>
+    <mergeCell ref="B109:C109"/>
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="B111:C111"/>
+    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="B113:C113"/>
+    <mergeCell ref="B114:C114"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="B116:C116"/>
+    <mergeCell ref="B117:C117"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="B103:C103"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="B93:C93"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="B98:C98"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5090,24 +5084,24 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1:BA1"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30" style="4" customWidth="1"/>
-    <col min="2" max="3" width="20" style="8" customWidth="1"/>
+    <col min="2" max="3" width="20" style="11" customWidth="1"/>
     <col min="4" max="53" width="20" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="10" t="s">
         <v>256</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="10" t="s">
         <v>257</v>
       </c>
       <c r="D1" s="5" t="s">
@@ -5261,14 +5255,14 @@
         <v>307</v>
       </c>
     </row>
-    <row r="2" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="10" t="s">
         <v>308</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="10" t="s">
         <v>308</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -5422,14 +5416,14 @@
         <v>308</v>
       </c>
     </row>
-    <row r="3" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="10" t="s">
         <v>310</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="10" t="s">
         <v>310</v>
       </c>
       <c r="D3" s="5" t="s">
@@ -5583,14 +5577,14 @@
         <v>310</v>
       </c>
     </row>
-    <row r="4" spans="1:53" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="11" t="s">
         <v>312</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="11" t="s">
         <v>313</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -5744,14 +5738,14 @@
         <v>363</v>
       </c>
     </row>
-    <row r="5" spans="1:53" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>364</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="11" t="s">
         <v>365</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="11" t="s">
         <v>368</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -5905,14 +5899,14 @@
         <v>441</v>
       </c>
     </row>
-    <row r="6" spans="1:53" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>442</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="11" t="s">
         <v>428</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="11" t="s">
         <v>385</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -6066,14 +6060,14 @@
         <v>427</v>
       </c>
     </row>
-    <row r="7" spans="1:53" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>460</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="11" t="s">
         <v>398</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="11" t="s">
         <v>390</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -6227,14 +6221,14 @@
         <v>481</v>
       </c>
     </row>
-    <row r="8" spans="1:53" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>485</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="11" t="s">
         <v>389</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="11" t="s">
         <v>431</v>
       </c>
       <c r="D8" s="4" t="s">
@@ -6388,14 +6382,14 @@
         <v>491</v>
       </c>
     </row>
-    <row r="9" spans="1:53" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>504</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="11" t="s">
         <v>452</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="11" t="s">
         <v>423</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -6549,14 +6543,14 @@
         <v>465</v>
       </c>
     </row>
-    <row r="10" spans="1:53" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>513</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="11" t="s">
         <v>514</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="11" t="s">
         <v>481</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -6710,14 +6704,14 @@
         <v>495</v>
       </c>
     </row>
-    <row r="11" spans="1:53" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>529</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="11" t="s">
         <v>497</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="11" t="s">
         <v>435</v>
       </c>
       <c r="D11" s="4" t="s">
@@ -6871,14 +6865,14 @@
         <v>432</v>
       </c>
     </row>
-    <row r="12" spans="1:53" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>531</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="11" t="s">
         <v>490</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="11" t="s">
         <v>527</v>
       </c>
       <c r="D12" s="4" t="s">
@@ -7032,14 +7026,14 @@
         <v>385</v>
       </c>
     </row>
-    <row r="13" spans="1:53" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>532</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="11" t="s">
         <v>380</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="11" t="s">
         <v>413</v>
       </c>
       <c r="D13" s="4" t="s">
@@ -7193,14 +7187,14 @@
         <v>382</v>
       </c>
     </row>
-    <row r="14" spans="1:53" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>533</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="11" t="s">
         <v>373</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="11" t="s">
         <v>438</v>
       </c>
       <c r="D14" s="4" t="s">
@@ -7354,175 +7348,175 @@
         <v>404</v>
       </c>
     </row>
-    <row r="15" spans="1:53" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
+    <row r="15" spans="1:53" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
         <v>535</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="11" t="s">
         <v>536</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="11" t="s">
         <v>537</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="11" t="s">
         <v>538</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="11" t="s">
         <v>539</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="11" t="s">
         <v>540</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="11" t="s">
         <v>541</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="H15" s="11" t="s">
         <v>542</v>
       </c>
-      <c r="I15" s="8" t="s">
+      <c r="I15" s="11" t="s">
         <v>543</v>
       </c>
-      <c r="J15" s="8" t="s">
+      <c r="J15" s="11" t="s">
         <v>544</v>
       </c>
-      <c r="K15" s="8" t="s">
+      <c r="K15" s="11" t="s">
         <v>545</v>
       </c>
-      <c r="L15" s="8" t="s">
+      <c r="L15" s="11" t="s">
         <v>546</v>
       </c>
-      <c r="M15" s="8" t="s">
+      <c r="M15" s="11" t="s">
         <v>547</v>
       </c>
-      <c r="N15" s="8" t="s">
+      <c r="N15" s="11" t="s">
         <v>548</v>
       </c>
-      <c r="O15" s="8" t="s">
+      <c r="O15" s="11" t="s">
         <v>549</v>
       </c>
-      <c r="P15" s="8" t="s">
+      <c r="P15" s="11" t="s">
         <v>550</v>
       </c>
-      <c r="Q15" s="8" t="s">
+      <c r="Q15" s="11" t="s">
         <v>551</v>
       </c>
-      <c r="R15" s="8" t="s">
+      <c r="R15" s="11" t="s">
         <v>552</v>
       </c>
-      <c r="S15" s="8" t="s">
+      <c r="S15" s="11" t="s">
         <v>553</v>
       </c>
-      <c r="T15" s="8" t="s">
+      <c r="T15" s="11" t="s">
         <v>554</v>
       </c>
-      <c r="U15" s="8" t="s">
+      <c r="U15" s="11" t="s">
         <v>555</v>
       </c>
-      <c r="V15" s="8" t="s">
+      <c r="V15" s="11" t="s">
         <v>556</v>
       </c>
-      <c r="W15" s="8" t="s">
+      <c r="W15" s="11" t="s">
         <v>557</v>
       </c>
-      <c r="X15" s="8" t="s">
+      <c r="X15" s="11" t="s">
         <v>558</v>
       </c>
-      <c r="Y15" s="8" t="s">
+      <c r="Y15" s="11" t="s">
         <v>559</v>
       </c>
-      <c r="Z15" s="8" t="s">
+      <c r="Z15" s="11" t="s">
         <v>560</v>
       </c>
-      <c r="AA15" s="8" t="s">
+      <c r="AA15" s="11" t="s">
         <v>561</v>
       </c>
-      <c r="AB15" s="8" t="s">
+      <c r="AB15" s="11" t="s">
         <v>562</v>
       </c>
-      <c r="AC15" s="8" t="s">
+      <c r="AC15" s="11" t="s">
         <v>563</v>
       </c>
-      <c r="AD15" s="8" t="s">
+      <c r="AD15" s="11" t="s">
         <v>564</v>
       </c>
-      <c r="AE15" s="8" t="s">
+      <c r="AE15" s="11" t="s">
         <v>565</v>
       </c>
-      <c r="AF15" s="8" t="s">
+      <c r="AF15" s="11" t="s">
         <v>566</v>
       </c>
-      <c r="AG15" s="8" t="s">
+      <c r="AG15" s="11" t="s">
         <v>567</v>
       </c>
-      <c r="AH15" s="8" t="s">
+      <c r="AH15" s="11" t="s">
         <v>568</v>
       </c>
-      <c r="AI15" s="8" t="s">
+      <c r="AI15" s="11" t="s">
         <v>569</v>
       </c>
-      <c r="AJ15" s="8" t="s">
+      <c r="AJ15" s="11" t="s">
         <v>570</v>
       </c>
-      <c r="AK15" s="8" t="s">
+      <c r="AK15" s="11" t="s">
         <v>571</v>
       </c>
-      <c r="AL15" s="8" t="s">
+      <c r="AL15" s="11" t="s">
         <v>572</v>
       </c>
-      <c r="AM15" s="8" t="s">
+      <c r="AM15" s="11" t="s">
         <v>573</v>
       </c>
-      <c r="AN15" s="8" t="s">
+      <c r="AN15" s="11" t="s">
         <v>574</v>
       </c>
-      <c r="AO15" s="8" t="s">
+      <c r="AO15" s="11" t="s">
         <v>575</v>
       </c>
-      <c r="AP15" s="8" t="s">
+      <c r="AP15" s="11" t="s">
         <v>576</v>
       </c>
-      <c r="AQ15" s="8" t="s">
+      <c r="AQ15" s="11" t="s">
         <v>577</v>
       </c>
-      <c r="AR15" s="8" t="s">
+      <c r="AR15" s="11" t="s">
         <v>578</v>
       </c>
-      <c r="AS15" s="8" t="s">
+      <c r="AS15" s="11" t="s">
         <v>579</v>
       </c>
-      <c r="AT15" s="8" t="s">
+      <c r="AT15" s="11" t="s">
         <v>580</v>
       </c>
-      <c r="AU15" s="8" t="s">
+      <c r="AU15" s="11" t="s">
         <v>581</v>
       </c>
-      <c r="AV15" s="8" t="s">
+      <c r="AV15" s="11" t="s">
         <v>582</v>
       </c>
-      <c r="AW15" s="8" t="s">
+      <c r="AW15" s="11" t="s">
         <v>583</v>
       </c>
-      <c r="AX15" s="8" t="s">
+      <c r="AX15" s="11" t="s">
         <v>584</v>
       </c>
-      <c r="AY15" s="8" t="s">
+      <c r="AY15" s="11" t="s">
         <v>585</v>
       </c>
-      <c r="AZ15" s="8" t="s">
+      <c r="AZ15" s="11" t="s">
         <v>586</v>
       </c>
-      <c r="BA15" s="8" t="s">
+      <c r="BA15" s="11" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="16" spans="1:53" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>588</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="11" t="s">
         <v>589</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="11" t="s">
         <v>590</v>
       </c>
       <c r="D16" s="4" t="s">
@@ -7676,19 +7670,19 @@
         <v>640</v>
       </c>
     </row>
-    <row r="17" spans="1:53" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>641</v>
       </c>
     </row>
-    <row r="18" spans="1:53" ht="32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>642</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="11" t="s">
         <v>643</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="11" t="s">
         <v>645</v>
       </c>
       <c r="D18" s="4" t="s">
@@ -7842,14 +7836,14 @@
         <v>682</v>
       </c>
     </row>
-    <row r="19" spans="1:53" ht="32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>683</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>644</v>
-      </c>
-      <c r="C19" s="8" t="s">
+      <c r="B19" s="11" t="s">
+        <v>644</v>
+      </c>
+      <c r="C19" s="11" t="s">
         <v>644</v>
       </c>
       <c r="D19" s="4" t="s">
@@ -8003,14 +7997,14 @@
         <v>644</v>
       </c>
     </row>
-    <row r="20" spans="1:53" ht="32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>684</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>644</v>
-      </c>
-      <c r="C20" s="8" t="s">
+      <c r="B20" s="11" t="s">
+        <v>644</v>
+      </c>
+      <c r="C20" s="11" t="s">
         <v>644</v>
       </c>
       <c r="D20" s="4" t="s">

</xml_diff>